<commit_message>
feat: add new query for sales
</commit_message>
<xml_diff>
--- a/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
+++ b/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Desafio1_DMD_EduardoLopez\Fiorella_Data_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Lopez\Documents\GitHub\desafio1_DMD_EduardoLopez\Fiorella_Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CB8341-3EE8-415D-87F0-B06920C03A9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E05C14D-BF5E-4442-AE6D-8206CBF60FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -348,13 +348,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" t="s">
@@ -532,174 +532,6 @@
         </is>
       </c>
     </row>
-    <row outlineLevel="0" r="16">
-      <c r="A16" s="0" t="inlineStr">
-        <is>
-          <t>Liston</t>
-        </is>
-      </c>
-      <c r="B16" s="0" t="inlineStr">
-        <is>
-          <t>975</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="17">
-      <c r="A17" s="0" t="inlineStr">
-        <is>
-          <t>Rosas</t>
-        </is>
-      </c>
-      <c r="B17" s="0" t="inlineStr">
-        <is>
-          <t>945</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="18">
-      <c r="A18" s="0" t="inlineStr">
-        <is>
-          <t>Globos</t>
-        </is>
-      </c>
-      <c r="B18" s="0" t="inlineStr">
-        <is>
-          <t>892</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="19">
-      <c r="A19" s="0" t="inlineStr">
-        <is>
-          <t>Aurora</t>
-        </is>
-      </c>
-      <c r="B19" s="0" t="inlineStr">
-        <is>
-          <t>804</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="20">
-      <c r="A20" s="0" t="inlineStr">
-        <is>
-          <t>Orquideas</t>
-        </is>
-      </c>
-      <c r="B20" s="0" t="inlineStr">
-        <is>
-          <t>797</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="21">
-      <c r="A21" s="0" t="inlineStr">
-        <is>
-          <t>Lirios</t>
-        </is>
-      </c>
-      <c r="B21" s="0" t="inlineStr">
-        <is>
-          <t>795</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="22">
-      <c r="A22" s="0" t="inlineStr">
-        <is>
-          <t>Girasoles</t>
-        </is>
-      </c>
-      <c r="B22" s="0" t="inlineStr">
-        <is>
-          <t>787</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="23">
-      <c r="A23" s="0" t="inlineStr">
-        <is>
-          <t>Tarjetas</t>
-        </is>
-      </c>
-      <c r="B23" s="0" t="inlineStr">
-        <is>
-          <t>779</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="24">
-      <c r="A24" s="0" t="inlineStr">
-        <is>
-          <t>Macetas</t>
-        </is>
-      </c>
-      <c r="B24" s="0" t="inlineStr">
-        <is>
-          <t>778</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="25">
-      <c r="A25" s="0" t="inlineStr">
-        <is>
-          <t>Hortensia</t>
-        </is>
-      </c>
-      <c r="B25" s="0" t="inlineStr">
-        <is>
-          <t>774</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="26">
-      <c r="A26" s="0" t="inlineStr">
-        <is>
-          <t>Tulipanes</t>
-        </is>
-      </c>
-      <c r="B26" s="0" t="inlineStr">
-        <is>
-          <t>753</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="27">
-      <c r="A27" s="0" t="inlineStr">
-        <is>
-          <t>Carmesi</t>
-        </is>
-      </c>
-      <c r="B27" s="0" t="inlineStr">
-        <is>
-          <t>747</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="28">
-      <c r="A28" s="0" t="inlineStr">
-        <is>
-          <t>Tierra</t>
-        </is>
-      </c>
-      <c r="B28" s="0" t="inlineStr">
-        <is>
-          <t>745</t>
-        </is>
-      </c>
-    </row>
-    <row outlineLevel="0" r="29">
-      <c r="A29" s="0" t="inlineStr">
-        <is>
-          <t>Claveles</t>
-        </is>
-      </c>
-      <c r="B29" s="0" t="inlineStr">
-        <is>
-          <t>733</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add new items to control flow for generating final xlsx files
</commit_message>
<xml_diff>
--- a/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
+++ b/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Lopez\Documents\GitHub\desafio1_DMD_EduardoLopez\Fiorella_Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E05C14D-BF5E-4442-AE6D-8206CBF60FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1C6B6B-2CC4-4B97-922E-69F0A33E3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: add final details and document
</commit_message>
<xml_diff>
--- a/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
+++ b/Fiorella_Data_Excel/Preferencia_Nacional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduardo Lopez\Documents\GitHub\desafio1_DMD_EduardoLopez\Fiorella_Data_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E1C6B6B-2CC4-4B97-922E-69F0A33E3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D80A27-788F-4636-8D5E-83C16A871F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A2" sqref="A2:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>